<commit_message>
update khung gia p1
</commit_message>
<xml_diff>
--- a/CSDLGia_ASP/wwwroot/UpLoad/File/DinhGia/Excel/FileExcelGiaSpDvKhungGia.xlsx
+++ b/CSDLGia_ASP/wwwroot/UpLoad/File/DinhGia/Excel/FileExcelGiaSpDvKhungGia.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CSDLGia_ASP\CSDLGia_ASP\wwwroot\UpLoad\File\DinhGia\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WEB\ASP\CSDLGia_ASP\CSDLGia_ASP\wwwroot\UpLoad\File\DinhGia\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{481B299F-B32F-45F7-A75D-3A510FAF8860}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C82111B9-3BA5-4EF8-BF73-E2F2200D6001}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6AF4210B-D7D1-451E-A048-5B80F2CEA5CC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6AF4210B-D7D1-451E-A048-5B80F2CEA5CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,43 +25,41 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
-  <si>
-    <t>Phân loại</t>
-  </si>
-  <si>
-    <t>Đơn vị</t>
-  </si>
-  <si>
-    <t>Mã nhóm</t>
-  </si>
-  <si>
-    <t>Tên nhóm</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Tàu cá cập cảng</t>
   </si>
   <si>
-    <t>Tàu có công suất dưới 20CV</t>
-  </si>
-  <si>
     <t>Đồng/Lần vào ra cảng</t>
   </si>
   <si>
-    <t>50000</t>
-  </si>
-  <si>
     <t>Giá tối thiểu</t>
   </si>
   <si>
     <t>Giá tối đa</t>
+  </si>
+  <si>
+    <t>STT</t>
+  </si>
+  <si>
+    <t>Đối tượng</t>
+  </si>
+  <si>
+    <t>Đơn vị tính</t>
+  </si>
+  <si>
+    <t>DANH SÁCH KHUNG GIÁ SẢN PHẨM DỊCH VỤ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -83,6 +81,22 @@
       <charset val="163"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="163"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="163"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -92,7 +106,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -100,31 +114,52 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -437,79 +472,81 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD0BC2B6-4560-4170-B0EA-9A729F87B874}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A2:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="24.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="34.5703125" customWidth="1"/>
-    <col min="4" max="4" width="25.7109375" customWidth="1"/>
-    <col min="5" max="6" width="38.42578125" customWidth="1"/>
-    <col min="7" max="7" width="19.140625" customWidth="1"/>
-    <col min="8" max="8" width="27.140625" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" customWidth="1"/>
+    <col min="4" max="5" width="38.42578125" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" customWidth="1"/>
+    <col min="7" max="7" width="27.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="2" spans="1:5" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+    </row>
+    <row r="3" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="E3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="4" t="s">
+    </row>
+    <row r="4" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
+        <v>1</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="C4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
-        <v>240130164808</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D4" s="9">
+        <v>100000</v>
+      </c>
+      <c r="E4" s="9">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
     </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:E2"/>
+  </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
khung giá - end
</commit_message>
<xml_diff>
--- a/CSDLGia_ASP/wwwroot/UpLoad/File/DinhGia/Excel/FileExcelGiaSpDvKhungGia.xlsx
+++ b/CSDLGia_ASP/wwwroot/UpLoad/File/DinhGia/Excel/FileExcelGiaSpDvKhungGia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WEB\ASP\CSDLGia_ASP\CSDLGia_ASP\wwwroot\UpLoad\File\DinhGia\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C82111B9-3BA5-4EF8-BF73-E2F2200D6001}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A6EFAD8-032E-4005-A91D-2763C52C14BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6AF4210B-D7D1-451E-A048-5B80F2CEA5CC}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Tàu cá cập cảng</t>
   </si>
@@ -49,6 +49,10 @@
   </si>
   <si>
     <t>DANH SÁCH KHUNG GIÁ SẢN PHẨM DỊCH VỤ</t>
+  </si>
+  <si>
+    <t>Mã nhóm sản phẩm
+(không có bỏ trống)</t>
   </si>
 </sst>
 </file>
@@ -57,7 +61,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -134,7 +138,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -153,10 +157,13 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -472,80 +479,89 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD0BC2B6-4560-4170-B0EA-9A729F87B874}">
-  <dimension ref="A2:E8"/>
+  <dimension ref="A2:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" customWidth="1"/>
-    <col min="4" max="5" width="38.42578125" customWidth="1"/>
-    <col min="6" max="6" width="19.140625" customWidth="1"/>
-    <col min="7" max="7" width="27.140625" customWidth="1"/>
+    <col min="1" max="2" width="11.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" customWidth="1"/>
+    <col min="5" max="6" width="38.42578125" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" customWidth="1"/>
+    <col min="8" max="8" width="27.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:6" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-    </row>
-    <row r="3" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+    </row>
+    <row r="3" spans="1:6" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="D3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="E3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="F3" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>1</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6"/>
+      <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="9">
+      <c r="E4" s="8">
         <v>100000</v>
       </c>
-      <c r="E4" s="9">
+      <c r="F4" s="8">
         <v>100000</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="2"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="2"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A2:F2"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>